<commit_message>
Atualização automática de SANTA_BARBARA_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/SANTA_BARBARA_DO_SUL.xlsx
+++ b/SANTA_BARBARA_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B976286-59DB-450C-AD15-2BC3C1477832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BB322F2-661F-4E00-8A91-56CB8EEB0C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1150,7 +1150,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{5A1DD0BA-A19E-4D1A-A14D-93AE94D30B59}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{3E892414-048B-4698-B0FE-2B28C51ED326}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1180,10 +1180,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B6E8744-C71B-42B6-89EE-347BFF24A6F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DD4B51-E904-47CA-BE53-79A0836E28E1}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1221,7 +1221,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{398BC15B-E638-4B64-ACB8-02DDCD7BFA7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{231910F2-91DC-4524-92CB-2143270D48FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1284,7 +1284,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E347257-A026-4123-9CE5-472D83C1B81A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61DA0385-BE5B-41FE-BE3D-BF57E3C8582D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1303,7 +1303,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9869826D-6FCB-08C0-6655-9BBD8A349D4F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4556AA9B-DEAF-C7D5-82AA-BB9B98FA5FC2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1352,7 +1352,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8911803C-374D-E514-20D7-68224E36FC9D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E784C1DE-A3D9-4F33-9B3E-6FD22A713C45}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1371,7 +1371,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{824BC8C4-83D5-B343-F279-2D38C35D4CA5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{499E52C2-E28E-D19A-6A5A-BF46C7ADACAC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1402,7 +1402,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDC37188-C613-8336-7DCD-FE5D19CB2071}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A9BB065-C3DD-0F6E-753E-481C099AD601}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF9E86AA-364B-4C63-C43D-D5B51F7C2E0F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F082B964-5286-5F61-A23B-55699175D887}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1476,7 +1476,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42EBEFE0-6576-457A-B024-2150DDCDF53F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FADEF427-95F5-4F4B-A9EA-62A71A05827B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1514,7 +1514,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B64B86F2-C8DE-4809-AC3E-B2C4206932A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26135956-BB71-4CD2-BF66-42A696AA817F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1557,7 +1557,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78FA5F52-C84D-4D42-9480-86158106DE09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87F81825-F18D-4DF2-B761-7C543B57EE1F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1870,7 +1870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05CB66B-A2B2-49C0-BAF1-87800D0F8798}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12674683-F646-4877-8BA5-A9D3F9861F45}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>